<commit_message>
Updates in module 2 and 4
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43F887-99FF-414D-AF66-C211CCDDC54E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF60345C-2E96-4DAB-8551-163705F93BD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ga1v+nrD6kb1AGYt8wD/rziE6kym7PE/tdi2hwaN1aQlQHlJf0916PcjCDIPire+kh0X4hlbY7Wz5sppGfMsDQ==" workbookSaltValue="6ijn1QT8HSXyqflHlvqmlw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="813">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2447,6 +2447,30 @@
   </si>
   <si>
     <t>Graduates By Ownership</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>1.2.5</t>
+  </si>
+  <si>
+    <t>1.2.6</t>
   </si>
 </sst>
 </file>
@@ -2783,9 +2807,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2804,6 +2825,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2815,15 +2839,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2838,6 +2853,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5341,7 +5365,7 @@
   <dimension ref="A1:BZ250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5754,8 +5778,8 @@
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>2</v>
+      <c r="B9" s="7" t="s">
+        <v>805</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>785</v>
@@ -5803,8 +5827,8 @@
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
-        <v>3</v>
+      <c r="B10" s="7" t="s">
+        <v>806</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>786</v>
@@ -5853,7 +5877,7 @@
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>5</v>
@@ -5902,7 +5926,7 @@
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
@@ -5951,7 +5975,7 @@
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>7</v>
@@ -6000,7 +6024,7 @@
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>8</v>
@@ -12210,7 +12234,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+jikH4mcinbT4Gb/XmZUZu7nnykqlifJmFjJgZE+kN/Gbife06lRlCAktSx3vhVmBNeNrcyIyXLVbbeZKTeOtQ==" saltValue="SEh8NlSuIN5+KAe5fZVSsQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/9rdoJayobbDEVqbt6/7at8no5HKbZEvDE906aUzP0PUYRpfDZyD7auZ3Aajrn1tWzuthKKceKq5QmA2YrotFw==" saltValue="MwJbHva1l9eaMMrsunq1tw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="L4 Q8:R15 M8:P14" name="Range1"/>
     <protectedRange sqref="D8:D11 D13:D14 E8:L14" name="Range1_1"/>
@@ -12409,9 +12433,9 @@
       </c>
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
       <c r="P6" s="12" t="s">
         <v>788</v>
       </c>
@@ -12453,9 +12477,9 @@
       <c r="K7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
       <c r="P7" s="12" t="s">
         <v>774</v>
       </c>
@@ -12467,235 +12491,235 @@
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
       <c r="P8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
-        <v>2</v>
+      <c r="B9" s="17" t="s">
+        <v>805</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>785</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
-        <v>3</v>
+      <c r="B10" s="17" t="s">
+        <v>806</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>786</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
       <c r="P10" s="12"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
-        <v>4</v>
-      </c>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="17" t="s">
+        <v>807</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>797</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
-        <v>5</v>
-      </c>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="17" t="s">
+        <v>808</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>798</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <v>6</v>
-      </c>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="17" t="s">
+        <v>809</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>799</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
-        <v>7</v>
-      </c>
-      <c r="C14" s="45" t="s">
+      <c r="B14" s="17" t="s">
+        <v>810</v>
+      </c>
+      <c r="C14" s="44" t="s">
         <v>800</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
-        <v>8</v>
-      </c>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="17" t="s">
+        <v>811</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>801</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
-        <v>9</v>
-      </c>
-      <c r="C16" s="45" t="s">
+      <c r="B16" s="17" t="s">
+        <v>812</v>
+      </c>
+      <c r="C16" s="44" t="s">
         <v>802</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="erWsy34Ypzz/jXwE9S5pRNG/MQdXY1H59b+YGM2GtPJD/E6rmw8VOAu7C71kbHfIlUTu7aCMG1uLpci4zEQLEA==" saltValue="i6TRbk03I38TCpZ9nk99Dg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ampibs05AMg9mkI14ADpiRP13jiyxBHbn8k6gC8WXR1sUIJhPPqXG9E7298083SvEBDi6GK495JIXAX6mODdeg==" saltValue="jTNUjqXH1NUbqoBI3OosDQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -12721,7 +12745,7 @@
   <dimension ref="B1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12831,29 +12855,29 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="56" t="s">
         <v>768</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="51" t="s">
         <v>794</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="51" t="s">
         <v>795</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="51" t="s">
         <v>796</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
       <c r="P6" s="12" t="s">
         <v>788</v>
       </c>
@@ -12871,166 +12895,166 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
       <c r="P7" s="12" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="40">
+      <c r="B8" s="46">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
       <c r="P8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="40">
-        <v>2</v>
+      <c r="B9" s="46" t="s">
+        <v>805</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>785</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40">
-        <v>3</v>
+      <c r="B10" s="46" t="s">
+        <v>806</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>786</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
       <c r="P10" s="12"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="40">
-        <v>4</v>
+      <c r="B11" s="46">
+        <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="40">
-        <v>5</v>
+      <c r="B12" s="46">
+        <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="40">
-        <v>6</v>
+      <c r="B13" s="46">
+        <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="40">
-        <v>7</v>
+      <c r="B14" s="46">
+        <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="54" t="s">
         <v>766</v>
       </c>
       <c r="D16" s="50" t="s">
@@ -13049,7 +13073,7 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="50"/>
-      <c r="C17" s="57"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
@@ -13067,18 +13091,18 @@
       <c r="C18" s="8" t="s">
         <v>803</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eeIfyLP+e1FTtxkr/wJ+2jC4GLK76Q7S9rh08pc5H0le3BXH4G048w2nmMKbVSb9cbRNsnO7j0etddlUiqQ1rQ==" saltValue="myLoyL1s9gVu5Frj1i8X9A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AVVNtKurxY+244LlqUO6Mr55Y+DsFtZ6pqnU2mBt056Phf+EUQd7kQqLoFJZG4bXAMbQGk1eGgGNiooBW0MAUg==" saltValue="LmsSR1eFF7lzbB5JJo3uyg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="13">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -13303,7 +13327,7 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="46">
         <v>1</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -13329,8 +13353,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>2</v>
+      <c r="B9" s="46" t="s">
+        <v>805</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>785</v>
@@ -13355,8 +13379,8 @@
       </c>
     </row>
     <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
-        <v>3</v>
+      <c r="B10" s="46" t="s">
+        <v>806</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>786</v>
@@ -13381,8 +13405,8 @@
       </c>
     </row>
     <row r="11" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <v>4</v>
+      <c r="B11" s="46">
+        <v>2</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>5</v>
@@ -13407,8 +13431,8 @@
       </c>
     </row>
     <row r="12" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>5</v>
+      <c r="B12" s="46">
+        <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>6</v>
@@ -13433,8 +13457,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
-        <v>6</v>
+      <c r="B13" s="46">
+        <v>4</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>7</v>
@@ -13459,8 +13483,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
-        <v>7</v>
+      <c r="B14" s="46">
+        <v>5</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>8</v>
@@ -14033,7 +14057,7 @@
       <c r="N50" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6UT2bMkgWY5yCW+qvPqylscy8UnBypDYlKnRB+v4DZIkUU2x7Aq8uJKvAGTFfONaiIjzbNEmzsYSwZ/WUex75w==" saltValue="WIbn73iD0kowtdi/yz5lJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AXmr4Buy5LNrHJIvifxdaCzTh2hoPCRz/P3NILYpwhCJPSNZbcK4vaUvLNoUQa8qCJt2gopG0F+6haPfjqOi0w==" saltValue="BzO3cEME+Y194hvvexLwEg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>

</xml_diff>

<commit_message>
Update modules 2 and 4
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF60345C-2E96-4DAB-8551-163705F93BD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB55409B-7A5D-4574-ADEE-4610D8D480E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ga1v+nrD6kb1AGYt8wD/rziE6kym7PE/tdi2hwaN1aQlQHlJf0916PcjCDIPire+kh0X4hlbY7Wz5sppGfMsDQ==" workbookSaltValue="6ijn1QT8HSXyqflHlvqmlw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2822,11 +2822,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12491,14 +12492,14 @@
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
       <c r="N8" s="42"/>
@@ -12513,14 +12514,14 @@
       <c r="C9" s="8" t="s">
         <v>785</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
@@ -12533,14 +12534,14 @@
       <c r="C10" s="8" t="s">
         <v>786</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
       <c r="N10" s="42"/>
@@ -12553,14 +12554,14 @@
       <c r="C11" s="44" t="s">
         <v>797</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
@@ -12572,14 +12573,14 @@
       <c r="C12" s="44" t="s">
         <v>798</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
       <c r="N12" s="42"/>
@@ -12591,14 +12592,14 @@
       <c r="C13" s="44" t="s">
         <v>799</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
@@ -12610,14 +12611,14 @@
       <c r="C14" s="44" t="s">
         <v>800</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
       <c r="L14" s="42"/>
       <c r="M14" s="42"/>
       <c r="N14" s="42"/>
@@ -12629,14 +12630,14 @@
       <c r="C15" s="44" t="s">
         <v>801</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -12645,14 +12646,14 @@
       <c r="C16" s="44" t="s">
         <v>802</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
@@ -12661,14 +12662,14 @@
       <c r="C17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
@@ -12677,14 +12678,14 @@
       <c r="C18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
@@ -12693,14 +12694,14 @@
       <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
@@ -12709,17 +12710,17 @@
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ampibs05AMg9mkI14ADpiRP13jiyxBHbn8k6gC8WXR1sUIJhPPqXG9E7298083SvEBDi6GK495JIXAX6mODdeg==" saltValue="jTNUjqXH1NUbqoBI3OosDQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2LZyqSrFpJCIsIMKtJS37r3a1lSEAIPnbfFv5y7lRk+PvjooqYCXP8nvr7iD1+lhzdy0LuNSe6R8pEHhc3a/fQ==" saltValue="pCWbfpeAIggHm4ciXTbFvw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -12731,7 +12732,7 @@
     <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:N14" xr:uid="{A3F639C4-71B1-403F-9979-D7791A6DEB32}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:N14 D8:K20" xr:uid="{A3F639C4-71B1-403F-9979-D7791A6DEB32}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -12745,7 +12746,7 @@
   <dimension ref="B1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12913,7 +12914,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -12935,7 +12936,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>805</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -12955,7 +12956,7 @@
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>806</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -12975,7 +12976,7 @@
       <c r="P10" s="12"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -12994,7 +12995,7 @@
       <c r="N11" s="42"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -13013,7 +13014,7 @@
       <c r="N12" s="42"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -13032,7 +13033,7 @@
       <c r="N13" s="42"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -13102,7 +13103,7 @@
       <c r="L18" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AVVNtKurxY+244LlqUO6Mr55Y+DsFtZ6pqnU2mBt056Phf+EUQd7kQqLoFJZG4bXAMbQGk1eGgGNiooBW0MAUg==" saltValue="LmsSR1eFF7lzbB5JJo3uyg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4/ok55WhQfb6Cp6MM/gwoVGtsyvYZhEH620akmq+x93iMyBgrnUq5Ok6X3XxzfCxhWrNTalgc/FI48BV7y9nSQ==" saltValue="tAybF8ONaHayJc5WYWl6+g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="13">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -13118,8 +13119,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:N14" xr:uid="{3F2DA1F0-36F6-4340-9093-2179365525C9}">
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:E14 G8:N14" xr:uid="{3F2DA1F0-36F6-4340-9093-2179365525C9}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F14" xr:uid="{3867CB6F-FFB9-4882-83A4-7CC1EF025656}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -13327,7 +13331,7 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>1</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -13353,7 +13357,7 @@
       </c>
     </row>
     <row r="9" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>805</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -13379,7 +13383,7 @@
       </c>
     </row>
     <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>806</v>
       </c>
       <c r="C10" s="20" t="s">
@@ -13405,7 +13409,7 @@
       </c>
     </row>
     <row r="11" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>2</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -13431,7 +13435,7 @@
       </c>
     </row>
     <row r="12" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
@@ -13457,7 +13461,7 @@
       </c>
     </row>
     <row r="13" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>4</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -13483,7 +13487,7 @@
       </c>
     </row>
     <row r="14" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>5</v>
       </c>
       <c r="C14" s="20" t="s">

</xml_diff>